<commit_message>
Update local authority data based on source changes
</commit_message>
<xml_diff>
--- a/docs/data/uk_la_future/1/uk_la_future.xlsx
+++ b/docs/data/uk_la_future/1/uk_la_future.xlsx
@@ -33,7 +33,7 @@
     <t>Dataset description</t>
   </si>
   <si>
-    <t xml:space="preserve">A dataset that include current and previous local authorities, as well as some planned but not in force yet
+    <t xml:space="preserve">A dataset that includes current and previous local authorities, as well as some planned but not in force yet
 </t>
   </si>
   <si>
@@ -46,7 +46,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Contributors</t>

</xml_diff>